<commit_message>
Exercícios de 26 a 30
</commit_message>
<xml_diff>
--- a/js.xlsx
+++ b/js.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="14115" windowHeight="7725" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="14115" windowHeight="7725" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comandos - JS" sheetId="4" r:id="rId1"/>
@@ -2805,6 +2805,120 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2814,124 +2928,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4057,7 +4057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -4407,7 +4407,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="165" t="s">
         <v>113</v>
       </c>
       <c r="B1" s="68">
@@ -4425,16 +4425,16 @@
       <c r="F1" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="129" t="s">
+      <c r="G1" s="149" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="131" t="s">
+      <c r="H1" s="167" t="s">
         <v>112</v>
       </c>
       <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="128"/>
+      <c r="A2" s="166"/>
       <c r="B2" s="66">
         <v>5</v>
       </c>
@@ -4450,12 +4450,12 @@
       <c r="F2" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="132"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="168"/>
       <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="128"/>
+      <c r="A3" s="166"/>
       <c r="B3" s="66">
         <v>5</v>
       </c>
@@ -4471,14 +4471,14 @@
       <c r="F3" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="132" t="s">
+      <c r="G3" s="150"/>
+      <c r="H3" s="168" t="s">
         <v>111</v>
       </c>
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
+      <c r="A4" s="166"/>
       <c r="B4" s="66">
         <v>5</v>
       </c>
@@ -4494,12 +4494,12 @@
       <c r="F4" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="G4" s="130"/>
-      <c r="H4" s="132"/>
+      <c r="G4" s="150"/>
+      <c r="H4" s="168"/>
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="128"/>
+      <c r="A5" s="166"/>
       <c r="B5" s="66">
         <v>5</v>
       </c>
@@ -4515,16 +4515,16 @@
       <c r="F5" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="130"/>
-      <c r="H5" s="132" t="s">
+      <c r="G5" s="150"/>
+      <c r="H5" s="168" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="126" t="s">
+      <c r="I5" s="164" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="128"/>
+      <c r="A6" s="166"/>
       <c r="B6" s="66">
         <v>5</v>
       </c>
@@ -4540,17 +4540,17 @@
       <c r="F6" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="G6" s="130"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="126"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="164"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="138"/>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="140"/>
+      <c r="A7" s="154"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="155"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="156"/>
       <c r="G7" s="31"/>
       <c r="H7" s="87" t="s">
         <v>109</v>
@@ -4558,14 +4558,14 @@
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="149" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="141"/>
       <c r="C8" s="141"/>
       <c r="D8" s="141"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="144" t="s">
+      <c r="E8" s="157"/>
+      <c r="F8" s="159" t="s">
         <v>183</v>
       </c>
       <c r="G8" s="86" t="s">
@@ -4577,7 +4577,7 @@
       <c r="I8" s="84"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
+      <c r="A9" s="150"/>
       <c r="B9" s="66" t="s">
         <v>180</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="E9" s="79">
         <v>8</v>
       </c>
-      <c r="F9" s="145"/>
+      <c r="F9" s="160"/>
       <c r="G9" s="81" t="s">
         <v>178</v>
       </c>
@@ -4598,7 +4598,7 @@
       <c r="I9" s="83"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="150"/>
       <c r="B10" s="66" t="s">
         <v>177</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="E10" s="79">
         <v>3</v>
       </c>
-      <c r="F10" s="145"/>
+      <c r="F10" s="160"/>
       <c r="G10" s="81" t="s">
         <v>175</v>
       </c>
@@ -4623,7 +4623,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
+      <c r="A11" s="150"/>
       <c r="B11" s="66" t="s">
         <v>172</v>
       </c>
@@ -4636,7 +4636,7 @@
       <c r="E11" s="79">
         <v>45</v>
       </c>
-      <c r="F11" s="145"/>
+      <c r="F11" s="160"/>
       <c r="G11" s="81" t="s">
         <v>170</v>
       </c>
@@ -4648,7 +4648,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
+      <c r="A12" s="150"/>
       <c r="B12" s="66" t="s">
         <v>167</v>
       </c>
@@ -4661,7 +4661,7 @@
       <c r="E12" s="79">
         <v>6</v>
       </c>
-      <c r="F12" s="145"/>
+      <c r="F12" s="160"/>
       <c r="G12" s="78" t="s">
         <v>165</v>
       </c>
@@ -4673,7 +4673,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="130"/>
+      <c r="A13" s="150"/>
       <c r="B13" s="66" t="s">
         <v>162</v>
       </c>
@@ -4686,7 +4686,7 @@
       <c r="E13" s="79">
         <v>2</v>
       </c>
-      <c r="F13" s="145"/>
+      <c r="F13" s="160"/>
       <c r="G13" s="78" t="s">
         <v>160</v>
       </c>
@@ -4698,7 +4698,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="130"/>
+      <c r="A14" s="150"/>
       <c r="B14" s="66" t="s">
         <v>157</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="E14" s="79">
         <v>3</v>
       </c>
-      <c r="F14" s="145"/>
+      <c r="F14" s="160"/>
       <c r="G14" s="78" t="s">
         <v>154</v>
       </c>
@@ -4723,12 +4723,12 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="130"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="140"/>
-      <c r="F15" s="146"/>
+      <c r="A15" s="150"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="161"/>
       <c r="G15" s="76" t="s">
         <v>151</v>
       </c>
@@ -4740,10 +4740,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="149" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="162" t="s">
         <v>144</v>
       </c>
       <c r="C16" s="72" t="s">
@@ -4759,8 +4759,8 @@
       <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="130"/>
-      <c r="B17" s="148"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="163"/>
       <c r="C17" s="70" t="s">
         <v>147</v>
       </c>
@@ -4774,8 +4774,8 @@
       <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="130"/>
-      <c r="B18" s="148"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="163"/>
       <c r="C18" s="70" t="s">
         <v>146</v>
       </c>
@@ -4789,8 +4789,8 @@
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="130"/>
-      <c r="B19" s="148"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="163"/>
       <c r="C19" s="70" t="s">
         <v>146</v>
       </c>
@@ -4804,10 +4804,10 @@
       <c r="I19" s="27"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="129" t="s">
+      <c r="A20" s="149" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="147" t="s">
+      <c r="B20" s="162" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="72" t="s">
@@ -4823,8 +4823,8 @@
       <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="130"/>
-      <c r="B21" s="148"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="163"/>
       <c r="C21" s="70" t="s">
         <v>143</v>
       </c>
@@ -4838,8 +4838,8 @@
       <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="130"/>
-      <c r="B22" s="148"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="163"/>
       <c r="C22" s="70" t="s">
         <v>139</v>
       </c>
@@ -4853,8 +4853,8 @@
       <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="130"/>
-      <c r="B23" s="148"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="163"/>
       <c r="C23" s="70" t="s">
         <v>141</v>
       </c>
@@ -4868,8 +4868,8 @@
       <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="130"/>
-      <c r="B24" s="148"/>
+      <c r="A24" s="150"/>
+      <c r="B24" s="163"/>
       <c r="C24" s="70" t="s">
         <v>139</v>
       </c>
@@ -4883,7 +4883,7 @@
       <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="149" t="s">
+      <c r="A25" s="131" t="s">
         <v>137</v>
       </c>
       <c r="B25" s="68">
@@ -4906,7 +4906,7 @@
       <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="150"/>
+      <c r="A26" s="132"/>
       <c r="B26" s="66">
         <v>7</v>
       </c>
@@ -4927,7 +4927,7 @@
       <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="150"/>
+      <c r="A27" s="132"/>
       <c r="B27" s="66">
         <v>8</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="150"/>
+      <c r="A28" s="132"/>
       <c r="B28" s="66">
         <v>9</v>
       </c>
@@ -4969,7 +4969,7 @@
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="150"/>
+      <c r="A29" s="132"/>
       <c r="B29" s="66">
         <v>5</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="150"/>
+      <c r="A30" s="132"/>
       <c r="B30" s="66">
         <v>4</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="150"/>
+      <c r="A31" s="132"/>
       <c r="B31" s="62">
         <v>5</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="151"/>
+      <c r="A32" s="133"/>
       <c r="B32" s="62">
         <v>5</v>
       </c>
@@ -5057,51 +5057,51 @@
       <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="163" t="s">
+      <c r="A33" s="143" t="s">
         <v>105</v>
       </c>
       <c r="B33" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="135" t="s">
+      <c r="C33" s="142" t="s">
         <v>104</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="167"/>
-      <c r="F33" s="133" t="s">
+      <c r="E33" s="152"/>
+      <c r="F33" s="146" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="129" t="s">
+      <c r="G33" s="149" t="s">
         <v>117</v>
       </c>
-      <c r="H33" s="135" t="s">
+      <c r="H33" s="142" t="s">
         <v>104</v>
       </c>
       <c r="I33" s="32"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="164"/>
+      <c r="A34" s="144"/>
       <c r="B34" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="137"/>
+      <c r="C34" s="151"/>
       <c r="D34" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="168"/>
-      <c r="F34" s="134"/>
-      <c r="G34" s="130"/>
-      <c r="H34" s="136"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="148"/>
+      <c r="G34" s="150"/>
+      <c r="H34" s="137"/>
       <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="164"/>
+      <c r="A35" s="144"/>
       <c r="B35" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="135" t="s">
+      <c r="C35" s="142" t="s">
         <v>103</v>
       </c>
       <c r="D35" s="54" t="s">
@@ -5110,72 +5110,72 @@
       <c r="E35" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="133" t="s">
+      <c r="F35" s="146" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="130"/>
-      <c r="H35" s="136" t="s">
+      <c r="G35" s="150"/>
+      <c r="H35" s="137" t="s">
         <v>103</v>
       </c>
       <c r="I35" s="27"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="164"/>
+      <c r="A36" s="144"/>
       <c r="B36" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="136"/>
+      <c r="C36" s="137"/>
       <c r="D36" s="50" t="s">
         <v>97</v>
       </c>
       <c r="E36" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="166"/>
-      <c r="G36" s="130"/>
-      <c r="H36" s="136"/>
+      <c r="F36" s="147"/>
+      <c r="G36" s="150"/>
+      <c r="H36" s="137"/>
       <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="164"/>
+      <c r="A37" s="144"/>
       <c r="B37" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="136"/>
+      <c r="C37" s="137"/>
       <c r="D37" s="52" t="s">
         <v>94</v>
       </c>
       <c r="E37" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="166"/>
-      <c r="G37" s="130"/>
-      <c r="H37" s="136"/>
+      <c r="F37" s="147"/>
+      <c r="G37" s="150"/>
+      <c r="H37" s="137"/>
       <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="164"/>
+      <c r="A38" s="144"/>
       <c r="B38" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="137"/>
+      <c r="C38" s="151"/>
       <c r="D38" s="56" t="s">
         <v>97</v>
       </c>
       <c r="E38" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="134"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="136"/>
+      <c r="F38" s="148"/>
+      <c r="G38" s="150"/>
+      <c r="H38" s="137"/>
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="164"/>
+      <c r="A39" s="144"/>
       <c r="B39" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="135" t="s">
+      <c r="C39" s="142" t="s">
         <v>102</v>
       </c>
       <c r="D39" s="54" t="s">
@@ -5184,71 +5184,71 @@
       <c r="E39" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="133" t="s">
+      <c r="F39" s="146" t="s">
         <v>115</v>
       </c>
-      <c r="G39" s="130"/>
-      <c r="H39" s="136" t="s">
+      <c r="G39" s="150"/>
+      <c r="H39" s="137" t="s">
         <v>102</v>
       </c>
       <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="164"/>
+      <c r="A40" s="144"/>
       <c r="B40" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="136"/>
+      <c r="C40" s="137"/>
       <c r="D40" s="50" t="s">
         <v>97</v>
       </c>
       <c r="E40" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="166"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="136"/>
+      <c r="F40" s="147"/>
+      <c r="G40" s="150"/>
+      <c r="H40" s="137"/>
       <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="164"/>
+      <c r="A41" s="144"/>
       <c r="B41" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="136"/>
+      <c r="C41" s="137"/>
       <c r="D41" s="52" t="s">
         <v>94</v>
       </c>
       <c r="E41" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="166"/>
-      <c r="G41" s="130"/>
-      <c r="H41" s="136"/>
+      <c r="F41" s="147"/>
+      <c r="G41" s="150"/>
+      <c r="H41" s="137"/>
       <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="165"/>
+      <c r="A42" s="145"/>
       <c r="B42" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="136"/>
+      <c r="C42" s="137"/>
       <c r="D42" s="50" t="s">
         <v>97</v>
       </c>
       <c r="E42" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="166"/>
-      <c r="G42" s="130"/>
-      <c r="H42" s="136"/>
+      <c r="F42" s="147"/>
+      <c r="G42" s="150"/>
+      <c r="H42" s="137"/>
       <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="152" t="s">
+      <c r="A43" s="126" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="160" t="s">
+      <c r="B43" s="138" t="s">
         <v>113</v>
       </c>
       <c r="C43" s="44" t="s">
@@ -5262,8 +5262,8 @@
       <c r="I43" s="32"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="153"/>
-      <c r="B44" s="161"/>
+      <c r="A44" s="127"/>
+      <c r="B44" s="139"/>
       <c r="C44" s="49" t="s">
         <v>111</v>
       </c>
@@ -5275,8 +5275,8 @@
       <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="153"/>
-      <c r="B45" s="161"/>
+      <c r="A45" s="127"/>
+      <c r="B45" s="139"/>
       <c r="C45" s="49" t="s">
         <v>110</v>
       </c>
@@ -5288,8 +5288,8 @@
       <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="153"/>
-      <c r="B46" s="162"/>
+      <c r="A46" s="127"/>
+      <c r="B46" s="140"/>
       <c r="C46" s="48" t="s">
         <v>109</v>
       </c>
@@ -5301,7 +5301,7 @@
       <c r="I46" s="24"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="153"/>
+      <c r="A47" s="127"/>
       <c r="B47" s="47" t="s">
         <v>108</v>
       </c>
@@ -5318,8 +5318,8 @@
       <c r="I47" s="32"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="153"/>
-      <c r="B48" s="157" t="s">
+      <c r="A48" s="127"/>
+      <c r="B48" s="134" t="s">
         <v>105</v>
       </c>
       <c r="C48" s="46" t="s">
@@ -5333,8 +5333,8 @@
       <c r="I48" s="32"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="153"/>
-      <c r="B49" s="158"/>
+      <c r="A49" s="127"/>
+      <c r="B49" s="135"/>
       <c r="C49" s="45" t="s">
         <v>103</v>
       </c>
@@ -5346,8 +5346,8 @@
       <c r="I49" s="27"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="154"/>
-      <c r="B50" s="159"/>
+      <c r="A50" s="128"/>
+      <c r="B50" s="136"/>
       <c r="C50" s="38" t="s">
         <v>102</v>
       </c>
@@ -5359,7 +5359,7 @@
       <c r="I50" s="24"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="149" t="s">
+      <c r="A51" s="131" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="44" t="s">
@@ -5382,7 +5382,7 @@
       <c r="I51" s="32"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="150"/>
+      <c r="A52" s="132"/>
       <c r="B52" s="39" t="s">
         <v>96</v>
       </c>
@@ -5399,7 +5399,7 @@
       <c r="I52" s="24"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="150"/>
+      <c r="A53" s="132"/>
       <c r="B53" s="35" t="s">
         <v>93</v>
       </c>
@@ -5412,11 +5412,11 @@
       <c r="I53" s="32"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="150"/>
-      <c r="B54" s="155" t="s">
+      <c r="A54" s="132"/>
+      <c r="B54" s="129" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="156"/>
+      <c r="C54" s="130"/>
       <c r="D54" s="28" t="s">
         <v>91</v>
       </c>
@@ -5427,7 +5427,7 @@
       <c r="I54" s="27"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="150"/>
+      <c r="A55" s="132"/>
       <c r="B55" s="26" t="s">
         <v>90</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="I55" s="24"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="150"/>
+      <c r="A56" s="132"/>
       <c r="B56" s="35" t="s">
         <v>89</v>
       </c>
@@ -5453,7 +5453,7 @@
       <c r="I56" s="32"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="150"/>
+      <c r="A57" s="132"/>
       <c r="B57" s="31" t="s">
         <v>88</v>
       </c>
@@ -5468,7 +5468,7 @@
       <c r="I57" s="27"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="151"/>
+      <c r="A58" s="133"/>
       <c r="B58" s="26" t="s">
         <v>86</v>
       </c>
@@ -5482,6 +5482,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="G1:G6"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A25:A32"/>
     <mergeCell ref="A43:A50"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="A51:A58"/>
@@ -5498,24 +5516,6 @@
     <mergeCell ref="H35:H38"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="G1:G6"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5526,7 +5526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="170"/>
-      <c r="B22" s="126"/>
+      <c r="B22" s="164"/>
       <c r="C22" s="174" t="s">
         <v>218</v>
       </c>
@@ -5847,7 +5847,7 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="170"/>
-      <c r="B23" s="126"/>
+      <c r="B23" s="164"/>
       <c r="C23" s="175"/>
       <c r="D23" s="175"/>
       <c r="E23" s="175"/>
@@ -5863,7 +5863,7 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="170"/>
-      <c r="B24" s="126"/>
+      <c r="B24" s="164"/>
       <c r="C24" s="172" t="s">
         <v>214</v>
       </c>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="170"/>
-      <c r="B25" s="126"/>
+      <c r="B25" s="164"/>
       <c r="C25" s="185" t="s">
         <v>211</v>
       </c>
@@ -5976,7 +5976,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="170"/>
-      <c r="B30" s="133" t="s">
+      <c r="B30" s="146" t="s">
         <v>200</v>
       </c>
       <c r="C30" s="181" t="s">
@@ -5996,7 +5996,7 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="171"/>
-      <c r="B31" s="134"/>
+      <c r="B31" s="148"/>
       <c r="C31" s="183" t="s">
         <v>197</v>
       </c>
@@ -6202,13 +6202,13 @@
       <c r="I3" s="90"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="149" t="s">
         <v>262</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="167" t="s">
         <v>261</v>
       </c>
-      <c r="C4" s="131" t="s">
+      <c r="C4" s="167" t="s">
         <v>260</v>
       </c>
       <c r="D4" s="33" t="s">
@@ -6223,9 +6223,9 @@
       <c r="I4" s="186"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="130"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
+      <c r="A5" s="150"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="168"/>
       <c r="D5" s="29" t="s">
         <v>257</v>
       </c>
@@ -6233,12 +6233,12 @@
       <c r="F5" s="194"/>
       <c r="G5" s="194"/>
       <c r="H5" s="194"/>
-      <c r="I5" s="126"/>
+      <c r="I5" s="164"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="132"/>
+      <c r="A6" s="150"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="168"/>
       <c r="D6" s="29" t="s">
         <v>253</v>
       </c>
@@ -6246,12 +6246,12 @@
       <c r="F6" s="194"/>
       <c r="G6" s="194"/>
       <c r="H6" s="194"/>
-      <c r="I6" s="126"/>
+      <c r="I6" s="164"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
+      <c r="A7" s="150"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="168"/>
       <c r="D7" s="113" t="s">
         <v>255</v>
       </c>
@@ -6259,12 +6259,12 @@
       <c r="F7" s="194"/>
       <c r="G7" s="194"/>
       <c r="H7" s="194"/>
-      <c r="I7" s="126"/>
+      <c r="I7" s="164"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
+      <c r="A8" s="150"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
       <c r="D8" s="29" t="s">
         <v>256</v>
       </c>
@@ -6272,12 +6272,12 @@
       <c r="F8" s="194"/>
       <c r="G8" s="194"/>
       <c r="H8" s="194"/>
-      <c r="I8" s="126"/>
+      <c r="I8" s="164"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
-      <c r="B9" s="132"/>
-      <c r="C9" s="132"/>
+      <c r="A9" s="150"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="168"/>
       <c r="D9" s="29" t="s">
         <v>253</v>
       </c>
@@ -6285,12 +6285,12 @@
       <c r="F9" s="194"/>
       <c r="G9" s="194"/>
       <c r="H9" s="194"/>
-      <c r="I9" s="126"/>
+      <c r="I9" s="164"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
-      <c r="B10" s="132"/>
-      <c r="C10" s="132"/>
+      <c r="A10" s="150"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="168"/>
       <c r="D10" s="113" t="s">
         <v>255</v>
       </c>
@@ -6298,12 +6298,12 @@
       <c r="F10" s="194"/>
       <c r="G10" s="194"/>
       <c r="H10" s="194"/>
-      <c r="I10" s="126"/>
+      <c r="I10" s="164"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
+      <c r="A11" s="150"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="168"/>
       <c r="D11" s="29" t="s">
         <v>254</v>
       </c>
@@ -6311,12 +6311,12 @@
       <c r="F11" s="194"/>
       <c r="G11" s="194"/>
       <c r="H11" s="194"/>
-      <c r="I11" s="126"/>
+      <c r="I11" s="164"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
+      <c r="A12" s="150"/>
+      <c r="B12" s="168"/>
+      <c r="C12" s="168"/>
       <c r="D12" s="29" t="s">
         <v>253</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="F12" s="194"/>
       <c r="G12" s="194"/>
       <c r="H12" s="194"/>
-      <c r="I12" s="126"/>
+      <c r="I12" s="164"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="192"/>

</xml_diff>

<commit_message>
update exercícios da Apostila
</commit_message>
<xml_diff>
--- a/js.xlsx
+++ b/js.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="14115" windowHeight="7725"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="14115" windowHeight="7725" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Comandos - JS" sheetId="4" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Eventos DOM" sheetId="8" r:id="rId5"/>
     <sheet name="Condições JS" sheetId="9" r:id="rId6"/>
     <sheet name="Funções ()" sheetId="10" r:id="rId7"/>
+    <sheet name="Repetições" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -195,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="305">
   <si>
     <t>0 a 6 - Domingo a Sábado</t>
   </si>
@@ -2041,6 +2042,54 @@
   </si>
   <si>
     <t>Mostrar na tela a imagem</t>
+  </si>
+  <si>
+    <t>While</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Repetição simples</t>
+  </si>
+  <si>
+    <t>Teste no início</t>
+  </si>
+  <si>
+    <t>var cont = 1</t>
+  </si>
+  <si>
+    <t>while(cont &lt;= 6){</t>
+  </si>
+  <si>
+    <t>    console.log(`Passo ${cont}`)</t>
+  </si>
+  <si>
+    <t>    cont++</t>
+  </si>
+  <si>
+    <t>Do While</t>
+  </si>
+  <si>
+    <t>}while(cont &lt;= 6)</t>
+  </si>
+  <si>
+    <t>do{</t>
+  </si>
+  <si>
+    <t>Teste no final</t>
+  </si>
+  <si>
+    <t>var num = Math.floor(Math.random()*10)+1</t>
+  </si>
+  <si>
+    <t>Número aleatório de 1 a 10</t>
+  </si>
+  <si>
+    <t>var num = Math.floor(Math.random()*11)</t>
+  </si>
+  <si>
+    <t>Número aleatório de 0 a 10</t>
   </si>
 </sst>
 </file>
@@ -2599,7 +2648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2857,6 +2906,37 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2878,6 +2958,84 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2893,15 +3051,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2911,9 +3060,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2923,12 +3069,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2938,75 +3078,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3088,30 +3168,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4026,7 +4113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -4140,10 +4227,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="127" t="s">
         <v>286</v>
       </c>
-      <c r="B11" s="200" t="s">
+      <c r="B11" s="122" t="s">
         <v>283</v>
       </c>
       <c r="C11" s="33" t="s">
@@ -4152,16 +4239,16 @@
       <c r="D11" s="32"/>
     </row>
     <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="202"/>
-      <c r="B12" s="201" t="s">
+      <c r="A12" s="128"/>
+      <c r="B12" s="123" t="s">
         <v>285</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="198"/>
-      <c r="B13" s="199" t="s">
+      <c r="A13" s="129"/>
+      <c r="B13" s="121" t="s">
         <v>287</v>
       </c>
       <c r="C13" s="25"/>
@@ -4170,7 +4257,7 @@
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="196"/>
+      <c r="B19" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4198,10 +4285,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="134" t="s">
         <v>84</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -4210,97 +4297,97 @@
       <c r="D1" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="125" t="s">
+      <c r="E1" s="136" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="121"/>
-      <c r="B2" s="123"/>
+      <c r="A2" s="132"/>
+      <c r="B2" s="134"/>
       <c r="C2" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="125"/>
+      <c r="E2" s="136"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="121"/>
-      <c r="B3" s="123"/>
+      <c r="A3" s="132"/>
+      <c r="B3" s="134"/>
       <c r="C3" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="125"/>
+      <c r="E3" s="136"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="121"/>
-      <c r="B4" s="123"/>
+      <c r="A4" s="132"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="125"/>
+      <c r="E4" s="136"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
-      <c r="B5" s="123"/>
+      <c r="A5" s="132"/>
+      <c r="B5" s="134"/>
       <c r="C5" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="124" t="s">
+      <c r="E5" s="135" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="121"/>
-      <c r="B6" s="123"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="124"/>
+      <c r="E6" s="135"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="121"/>
-      <c r="B7" s="123"/>
+      <c r="A7" s="132"/>
+      <c r="B7" s="134"/>
       <c r="C7" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="124"/>
+      <c r="E7" s="135"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
-      <c r="B8" s="123"/>
+      <c r="A8" s="132"/>
+      <c r="B8" s="134"/>
       <c r="C8" s="7"/>
       <c r="D8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="119" t="s">
+      <c r="E8" s="130" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="123"/>
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="7"/>
       <c r="D9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="119"/>
+      <c r="E9" s="130"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -4535,7 +4622,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="138" t="s">
         <v>113</v>
       </c>
       <c r="B1" s="68">
@@ -4553,16 +4640,16 @@
       <c r="F1" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="149" t="s">
+      <c r="G1" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="167" t="s">
+      <c r="H1" s="142" t="s">
         <v>112</v>
       </c>
       <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="166"/>
+      <c r="A2" s="139"/>
       <c r="B2" s="66">
         <v>5</v>
       </c>
@@ -4578,12 +4665,12 @@
       <c r="F2" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="150"/>
-      <c r="H2" s="168"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="143"/>
       <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="166"/>
+      <c r="A3" s="139"/>
       <c r="B3" s="66">
         <v>5</v>
       </c>
@@ -4599,14 +4686,14 @@
       <c r="F3" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="150"/>
-      <c r="H3" s="168" t="s">
+      <c r="G3" s="141"/>
+      <c r="H3" s="143" t="s">
         <v>111</v>
       </c>
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="166"/>
+      <c r="A4" s="139"/>
       <c r="B4" s="66">
         <v>5</v>
       </c>
@@ -4622,12 +4709,12 @@
       <c r="F4" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="G4" s="150"/>
-      <c r="H4" s="168"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="143"/>
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="166"/>
+      <c r="A5" s="139"/>
       <c r="B5" s="66">
         <v>5</v>
       </c>
@@ -4643,16 +4730,16 @@
       <c r="F5" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="150"/>
-      <c r="H5" s="168" t="s">
+      <c r="G5" s="141"/>
+      <c r="H5" s="143" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="164" t="s">
+      <c r="I5" s="137" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="166"/>
+      <c r="A6" s="139"/>
       <c r="B6" s="66">
         <v>5</v>
       </c>
@@ -4668,17 +4755,17 @@
       <c r="F6" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="G6" s="150"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="164"/>
+      <c r="G6" s="141"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="137"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="154"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="156"/>
+      <c r="A7" s="149"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="151"/>
       <c r="G7" s="31"/>
       <c r="H7" s="87" t="s">
         <v>109</v>
@@ -4686,14 +4773,14 @@
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="149" t="s">
+      <c r="A8" s="140" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="141"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="159" t="s">
+      <c r="B8" s="152"/>
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="155" t="s">
         <v>183</v>
       </c>
       <c r="G8" s="86" t="s">
@@ -4705,7 +4792,7 @@
       <c r="I8" s="84"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="150"/>
+      <c r="A9" s="141"/>
       <c r="B9" s="66" t="s">
         <v>180</v>
       </c>
@@ -4718,7 +4805,7 @@
       <c r="E9" s="79">
         <v>8</v>
       </c>
-      <c r="F9" s="160"/>
+      <c r="F9" s="156"/>
       <c r="G9" s="81" t="s">
         <v>178</v>
       </c>
@@ -4726,7 +4813,7 @@
       <c r="I9" s="83"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="150"/>
+      <c r="A10" s="141"/>
       <c r="B10" s="66" t="s">
         <v>177</v>
       </c>
@@ -4739,7 +4826,7 @@
       <c r="E10" s="79">
         <v>3</v>
       </c>
-      <c r="F10" s="160"/>
+      <c r="F10" s="156"/>
       <c r="G10" s="81" t="s">
         <v>175</v>
       </c>
@@ -4751,7 +4838,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="150"/>
+      <c r="A11" s="141"/>
       <c r="B11" s="66" t="s">
         <v>172</v>
       </c>
@@ -4764,7 +4851,7 @@
       <c r="E11" s="79">
         <v>45</v>
       </c>
-      <c r="F11" s="160"/>
+      <c r="F11" s="156"/>
       <c r="G11" s="81" t="s">
         <v>170</v>
       </c>
@@ -4776,7 +4863,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
+      <c r="A12" s="141"/>
       <c r="B12" s="66" t="s">
         <v>167</v>
       </c>
@@ -4789,7 +4876,7 @@
       <c r="E12" s="79">
         <v>6</v>
       </c>
-      <c r="F12" s="160"/>
+      <c r="F12" s="156"/>
       <c r="G12" s="78" t="s">
         <v>165</v>
       </c>
@@ -4801,7 +4888,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="150"/>
+      <c r="A13" s="141"/>
       <c r="B13" s="66" t="s">
         <v>162</v>
       </c>
@@ -4814,7 +4901,7 @@
       <c r="E13" s="79">
         <v>2</v>
       </c>
-      <c r="F13" s="160"/>
+      <c r="F13" s="156"/>
       <c r="G13" s="78" t="s">
         <v>160</v>
       </c>
@@ -4826,7 +4913,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="150"/>
+      <c r="A14" s="141"/>
       <c r="B14" s="66" t="s">
         <v>157</v>
       </c>
@@ -4839,7 +4926,7 @@
       <c r="E14" s="79">
         <v>3</v>
       </c>
-      <c r="F14" s="160"/>
+      <c r="F14" s="156"/>
       <c r="G14" s="78" t="s">
         <v>154</v>
       </c>
@@ -4851,12 +4938,12 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="150"/>
-      <c r="B15" s="158"/>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="156"/>
-      <c r="F15" s="161"/>
+      <c r="A15" s="141"/>
+      <c r="B15" s="154"/>
+      <c r="C15" s="154"/>
+      <c r="D15" s="154"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="157"/>
       <c r="G15" s="76" t="s">
         <v>151</v>
       </c>
@@ -4868,10 +4955,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="149" t="s">
+      <c r="A16" s="140" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="158" t="s">
         <v>144</v>
       </c>
       <c r="C16" s="72" t="s">
@@ -4887,8 +4974,8 @@
       <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
-      <c r="B17" s="163"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="70" t="s">
         <v>147</v>
       </c>
@@ -4902,8 +4989,8 @@
       <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="163"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="159"/>
       <c r="C18" s="70" t="s">
         <v>146</v>
       </c>
@@ -4917,8 +5004,8 @@
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="150"/>
-      <c r="B19" s="163"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="159"/>
       <c r="C19" s="70" t="s">
         <v>146</v>
       </c>
@@ -4932,10 +5019,10 @@
       <c r="I19" s="27"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="149" t="s">
+      <c r="A20" s="140" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="162" t="s">
+      <c r="B20" s="158" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="72" t="s">
@@ -4951,8 +5038,8 @@
       <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
-      <c r="B21" s="163"/>
+      <c r="A21" s="141"/>
+      <c r="B21" s="159"/>
       <c r="C21" s="70" t="s">
         <v>143</v>
       </c>
@@ -4966,8 +5053,8 @@
       <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="163"/>
+      <c r="A22" s="141"/>
+      <c r="B22" s="159"/>
       <c r="C22" s="70" t="s">
         <v>139</v>
       </c>
@@ -4981,8 +5068,8 @@
       <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="163"/>
+      <c r="A23" s="141"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="70" t="s">
         <v>141</v>
       </c>
@@ -4996,8 +5083,8 @@
       <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="150"/>
-      <c r="B24" s="163"/>
+      <c r="A24" s="141"/>
+      <c r="B24" s="159"/>
       <c r="C24" s="70" t="s">
         <v>139</v>
       </c>
@@ -5011,7 +5098,7 @@
       <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="131" t="s">
+      <c r="A25" s="160" t="s">
         <v>137</v>
       </c>
       <c r="B25" s="68">
@@ -5034,7 +5121,7 @@
       <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="132"/>
+      <c r="A26" s="161"/>
       <c r="B26" s="66">
         <v>7</v>
       </c>
@@ -5055,7 +5142,7 @@
       <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="132"/>
+      <c r="A27" s="161"/>
       <c r="B27" s="66">
         <v>8</v>
       </c>
@@ -5076,7 +5163,7 @@
       <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="132"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="66">
         <v>9</v>
       </c>
@@ -5097,7 +5184,7 @@
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="132"/>
+      <c r="A29" s="161"/>
       <c r="B29" s="66">
         <v>5</v>
       </c>
@@ -5118,7 +5205,7 @@
       <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="132"/>
+      <c r="A30" s="161"/>
       <c r="B30" s="66">
         <v>4</v>
       </c>
@@ -5139,7 +5226,7 @@
       <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="132"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="62">
         <v>5</v>
       </c>
@@ -5162,7 +5249,7 @@
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="133"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="62">
         <v>5</v>
       </c>
@@ -5185,51 +5272,51 @@
       <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="143" t="s">
+      <c r="A33" s="174" t="s">
         <v>105</v>
       </c>
       <c r="B33" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="142" t="s">
+      <c r="C33" s="146" t="s">
         <v>104</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="152"/>
-      <c r="F33" s="146" t="s">
+      <c r="E33" s="178"/>
+      <c r="F33" s="144" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="149" t="s">
+      <c r="G33" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="H33" s="142" t="s">
+      <c r="H33" s="146" t="s">
         <v>104</v>
       </c>
       <c r="I33" s="32"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="144"/>
+      <c r="A34" s="175"/>
       <c r="B34" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="151"/>
+      <c r="C34" s="148"/>
       <c r="D34" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="153"/>
-      <c r="F34" s="148"/>
-      <c r="G34" s="150"/>
-      <c r="H34" s="137"/>
+      <c r="E34" s="179"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="141"/>
+      <c r="H34" s="147"/>
       <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
+      <c r="A35" s="175"/>
       <c r="B35" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="142" t="s">
+      <c r="C35" s="146" t="s">
         <v>103</v>
       </c>
       <c r="D35" s="54" t="s">
@@ -5238,72 +5325,72 @@
       <c r="E35" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="146" t="s">
+      <c r="F35" s="144" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="150"/>
-      <c r="H35" s="137" t="s">
+      <c r="G35" s="141"/>
+      <c r="H35" s="147" t="s">
         <v>103</v>
       </c>
       <c r="I35" s="27"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
+      <c r="A36" s="175"/>
       <c r="B36" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="137"/>
+      <c r="C36" s="147"/>
       <c r="D36" s="50" t="s">
         <v>97</v>
       </c>
       <c r="E36" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="147"/>
-      <c r="G36" s="150"/>
-      <c r="H36" s="137"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="141"/>
+      <c r="H36" s="147"/>
       <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
+      <c r="A37" s="175"/>
       <c r="B37" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="137"/>
+      <c r="C37" s="147"/>
       <c r="D37" s="52" t="s">
         <v>94</v>
       </c>
       <c r="E37" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="147"/>
-      <c r="G37" s="150"/>
-      <c r="H37" s="137"/>
+      <c r="F37" s="177"/>
+      <c r="G37" s="141"/>
+      <c r="H37" s="147"/>
       <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="144"/>
+      <c r="A38" s="175"/>
       <c r="B38" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="151"/>
+      <c r="C38" s="148"/>
       <c r="D38" s="56" t="s">
         <v>97</v>
       </c>
       <c r="E38" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="148"/>
-      <c r="G38" s="150"/>
-      <c r="H38" s="137"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="141"/>
+      <c r="H38" s="147"/>
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
+      <c r="A39" s="175"/>
       <c r="B39" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="142" t="s">
+      <c r="C39" s="146" t="s">
         <v>102</v>
       </c>
       <c r="D39" s="54" t="s">
@@ -5312,71 +5399,71 @@
       <c r="E39" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="146" t="s">
+      <c r="F39" s="144" t="s">
         <v>115</v>
       </c>
-      <c r="G39" s="150"/>
-      <c r="H39" s="137" t="s">
+      <c r="G39" s="141"/>
+      <c r="H39" s="147" t="s">
         <v>102</v>
       </c>
       <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
+      <c r="A40" s="175"/>
       <c r="B40" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="137"/>
+      <c r="C40" s="147"/>
       <c r="D40" s="50" t="s">
         <v>97</v>
       </c>
       <c r="E40" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="147"/>
-      <c r="G40" s="150"/>
-      <c r="H40" s="137"/>
+      <c r="F40" s="177"/>
+      <c r="G40" s="141"/>
+      <c r="H40" s="147"/>
       <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
+      <c r="A41" s="175"/>
       <c r="B41" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="137"/>
+      <c r="C41" s="147"/>
       <c r="D41" s="52" t="s">
         <v>94</v>
       </c>
       <c r="E41" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="147"/>
-      <c r="G41" s="150"/>
-      <c r="H41" s="137"/>
+      <c r="F41" s="177"/>
+      <c r="G41" s="141"/>
+      <c r="H41" s="147"/>
       <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="145"/>
+      <c r="A42" s="176"/>
       <c r="B42" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="137"/>
+      <c r="C42" s="147"/>
       <c r="D42" s="50" t="s">
         <v>97</v>
       </c>
       <c r="E42" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="147"/>
-      <c r="G42" s="150"/>
-      <c r="H42" s="137"/>
+      <c r="F42" s="177"/>
+      <c r="G42" s="141"/>
+      <c r="H42" s="147"/>
       <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="126" t="s">
+      <c r="A43" s="163" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="138" t="s">
+      <c r="B43" s="171" t="s">
         <v>113</v>
       </c>
       <c r="C43" s="44" t="s">
@@ -5390,8 +5477,8 @@
       <c r="I43" s="32"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="127"/>
-      <c r="B44" s="139"/>
+      <c r="A44" s="164"/>
+      <c r="B44" s="172"/>
       <c r="C44" s="49" t="s">
         <v>111</v>
       </c>
@@ -5403,8 +5490,8 @@
       <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="127"/>
-      <c r="B45" s="139"/>
+      <c r="A45" s="164"/>
+      <c r="B45" s="172"/>
       <c r="C45" s="49" t="s">
         <v>110</v>
       </c>
@@ -5416,8 +5503,8 @@
       <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="127"/>
-      <c r="B46" s="140"/>
+      <c r="A46" s="164"/>
+      <c r="B46" s="173"/>
       <c r="C46" s="48" t="s">
         <v>109</v>
       </c>
@@ -5429,25 +5516,25 @@
       <c r="I46" s="24"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="127"/>
+      <c r="A47" s="164"/>
       <c r="B47" s="47" t="s">
         <v>108</v>
       </c>
       <c r="C47" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="141" t="s">
+      <c r="D47" s="152" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="141"/>
-      <c r="F47" s="141"/>
-      <c r="G47" s="141"/>
+      <c r="E47" s="152"/>
+      <c r="F47" s="152"/>
+      <c r="G47" s="152"/>
       <c r="H47" s="33"/>
       <c r="I47" s="32"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="127"/>
-      <c r="B48" s="134" t="s">
+      <c r="A48" s="164"/>
+      <c r="B48" s="168" t="s">
         <v>105</v>
       </c>
       <c r="C48" s="46" t="s">
@@ -5461,8 +5548,8 @@
       <c r="I48" s="32"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="127"/>
-      <c r="B49" s="135"/>
+      <c r="A49" s="164"/>
+      <c r="B49" s="169"/>
       <c r="C49" s="45" t="s">
         <v>103</v>
       </c>
@@ -5474,8 +5561,8 @@
       <c r="I49" s="27"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="128"/>
-      <c r="B50" s="136"/>
+      <c r="A50" s="165"/>
+      <c r="B50" s="170"/>
       <c r="C50" s="38" t="s">
         <v>102</v>
       </c>
@@ -5487,7 +5574,7 @@
       <c r="I50" s="24"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="131" t="s">
+      <c r="A51" s="160" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="44" t="s">
@@ -5510,7 +5597,7 @@
       <c r="I51" s="32"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="132"/>
+      <c r="A52" s="161"/>
       <c r="B52" s="39" t="s">
         <v>96</v>
       </c>
@@ -5527,7 +5614,7 @@
       <c r="I52" s="24"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="132"/>
+      <c r="A53" s="161"/>
       <c r="B53" s="35" t="s">
         <v>93</v>
       </c>
@@ -5540,11 +5627,11 @@
       <c r="I53" s="32"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="132"/>
-      <c r="B54" s="129" t="s">
+      <c r="A54" s="161"/>
+      <c r="B54" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="130"/>
+      <c r="C54" s="167"/>
       <c r="D54" s="28" t="s">
         <v>91</v>
       </c>
@@ -5555,7 +5642,7 @@
       <c r="I54" s="27"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="132"/>
+      <c r="A55" s="161"/>
       <c r="B55" s="26" t="s">
         <v>90</v>
       </c>
@@ -5568,7 +5655,7 @@
       <c r="I55" s="24"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="132"/>
+      <c r="A56" s="161"/>
       <c r="B56" s="35" t="s">
         <v>89</v>
       </c>
@@ -5581,7 +5668,7 @@
       <c r="I56" s="32"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="132"/>
+      <c r="A57" s="161"/>
       <c r="B57" s="31" t="s">
         <v>88</v>
       </c>
@@ -5596,7 +5683,7 @@
       <c r="I57" s="27"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="133"/>
+      <c r="A58" s="162"/>
       <c r="B58" s="26" t="s">
         <v>86</v>
       </c>
@@ -5610,24 +5697,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="G1:G6"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A25:A32"/>
     <mergeCell ref="A43:A50"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="A51:A58"/>
@@ -5644,6 +5713,24 @@
     <mergeCell ref="H35:H38"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="G1:G6"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5672,28 +5759,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="187" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="178"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="189"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="35"/>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
-      <c r="E2" s="173" t="s">
+      <c r="E2" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
@@ -5933,35 +6020,35 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="169" t="s">
+      <c r="A21" s="180" t="s">
         <v>221</v>
       </c>
-      <c r="B21" s="186" t="s">
+      <c r="B21" s="197" t="s">
         <v>220</v>
       </c>
-      <c r="C21" s="179" t="s">
+      <c r="C21" s="190" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="172"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="172"/>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172"/>
-      <c r="J21" s="172"/>
-      <c r="K21" s="172"/>
-      <c r="L21" s="180"/>
+      <c r="D21" s="183"/>
+      <c r="E21" s="183"/>
+      <c r="F21" s="183"/>
+      <c r="G21" s="183"/>
+      <c r="H21" s="183"/>
+      <c r="I21" s="183"/>
+      <c r="J21" s="183"/>
+      <c r="K21" s="183"/>
+      <c r="L21" s="191"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="170"/>
-      <c r="B22" s="164"/>
-      <c r="C22" s="174" t="s">
+      <c r="A22" s="181"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="185" t="s">
         <v>218</v>
       </c>
-      <c r="D22" s="174"/>
-      <c r="E22" s="174"/>
-      <c r="F22" s="174"/>
-      <c r="G22" s="174"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="185"/>
+      <c r="F22" s="185"/>
+      <c r="G22" s="185"/>
       <c r="H22" s="99" t="s">
         <v>217</v>
       </c>
@@ -5974,13 +6061,13 @@
       <c r="M22" s="93"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="170"/>
-      <c r="B23" s="164"/>
-      <c r="C23" s="175"/>
-      <c r="D23" s="175"/>
-      <c r="E23" s="175"/>
-      <c r="F23" s="175"/>
-      <c r="G23" s="175"/>
+      <c r="A23" s="181"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="186"/>
+      <c r="D23" s="186"/>
+      <c r="E23" s="186"/>
+      <c r="F23" s="186"/>
+      <c r="G23" s="186"/>
       <c r="H23" s="25" t="s">
         <v>215</v>
       </c>
@@ -5990,15 +6077,15 @@
       <c r="L23" s="96"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="170"/>
-      <c r="B24" s="164"/>
-      <c r="C24" s="172" t="s">
+      <c r="A24" s="181"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="183" t="s">
         <v>214</v>
       </c>
-      <c r="D24" s="172"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="172"/>
+      <c r="D24" s="183"/>
+      <c r="E24" s="183"/>
+      <c r="F24" s="183"/>
+      <c r="G24" s="183"/>
       <c r="H24" s="92" t="s">
         <v>213</v>
       </c>
@@ -6011,15 +6098,15 @@
       <c r="M24" s="93"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="170"/>
-      <c r="B25" s="164"/>
-      <c r="C25" s="185" t="s">
+      <c r="A25" s="181"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="196" t="s">
         <v>211</v>
       </c>
-      <c r="D25" s="185"/>
-      <c r="E25" s="185"/>
-      <c r="F25" s="185"/>
-      <c r="G25" s="185"/>
+      <c r="D25" s="196"/>
+      <c r="E25" s="196"/>
+      <c r="F25" s="196"/>
+      <c r="G25" s="196"/>
       <c r="H25" s="92" t="s">
         <v>210</v>
       </c>
@@ -6029,15 +6116,15 @@
       <c r="L25" s="90"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="170"/>
-      <c r="B26" s="187"/>
-      <c r="C26" s="185" t="s">
+      <c r="A26" s="181"/>
+      <c r="B26" s="198"/>
+      <c r="C26" s="196" t="s">
         <v>209</v>
       </c>
-      <c r="D26" s="185"/>
-      <c r="E26" s="185"/>
-      <c r="F26" s="185"/>
-      <c r="G26" s="185"/>
+      <c r="D26" s="196"/>
+      <c r="E26" s="196"/>
+      <c r="F26" s="196"/>
+      <c r="G26" s="196"/>
       <c r="H26" s="92" t="s">
         <v>208</v>
       </c>
@@ -6049,68 +6136,68 @@
       <c r="L26" s="90"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="170"/>
+      <c r="A27" s="181"/>
       <c r="B27" s="91" t="s">
         <v>206</v>
       </c>
-      <c r="C27" s="179" t="s">
+      <c r="C27" s="190" t="s">
         <v>205</v>
       </c>
-      <c r="D27" s="172"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="172"/>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="172"/>
-      <c r="K27" s="172"/>
-      <c r="L27" s="180"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="183"/>
+      <c r="F27" s="183"/>
+      <c r="G27" s="183"/>
+      <c r="H27" s="183"/>
+      <c r="I27" s="183"/>
+      <c r="J27" s="183"/>
+      <c r="K27" s="183"/>
+      <c r="L27" s="191"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="170"/>
+      <c r="A28" s="181"/>
       <c r="B28" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="C28" s="179" t="s">
+      <c r="C28" s="190" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="172"/>
-      <c r="E28" s="172"/>
-      <c r="F28" s="172"/>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="172"/>
-      <c r="J28" s="172"/>
-      <c r="K28" s="172"/>
-      <c r="L28" s="180"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="183"/>
+      <c r="F28" s="183"/>
+      <c r="G28" s="183"/>
+      <c r="H28" s="183"/>
+      <c r="I28" s="183"/>
+      <c r="J28" s="183"/>
+      <c r="K28" s="183"/>
+      <c r="L28" s="191"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="170"/>
+      <c r="A29" s="181"/>
       <c r="B29" s="90" t="s">
         <v>202</v>
       </c>
-      <c r="C29" s="179" t="s">
+      <c r="C29" s="190" t="s">
         <v>201</v>
       </c>
-      <c r="D29" s="172"/>
-      <c r="E29" s="172"/>
-      <c r="F29" s="172"/>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="172"/>
-      <c r="K29" s="172"/>
-      <c r="L29" s="180"/>
+      <c r="D29" s="183"/>
+      <c r="E29" s="183"/>
+      <c r="F29" s="183"/>
+      <c r="G29" s="183"/>
+      <c r="H29" s="183"/>
+      <c r="I29" s="183"/>
+      <c r="J29" s="183"/>
+      <c r="K29" s="183"/>
+      <c r="L29" s="191"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="170"/>
-      <c r="B30" s="146" t="s">
+      <c r="A30" s="181"/>
+      <c r="B30" s="144" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="181" t="s">
+      <c r="C30" s="192" t="s">
         <v>199</v>
       </c>
-      <c r="D30" s="182"/>
+      <c r="D30" s="193"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -6123,12 +6210,12 @@
       <c r="L30" s="32"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="171"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="183" t="s">
+      <c r="A31" s="182"/>
+      <c r="B31" s="145"/>
+      <c r="C31" s="194" t="s">
         <v>197</v>
       </c>
-      <c r="D31" s="184"/>
+      <c r="D31" s="195"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
@@ -6176,21 +6263,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="190" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172" t="s">
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="172"/>
-      <c r="F1" s="180"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="191"/>
       <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="188" t="s">
+      <c r="A3" s="199" t="s">
         <v>249</v>
       </c>
       <c r="B3" s="111" t="s">
@@ -6201,7 +6288,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="189"/>
+      <c r="A4" s="200"/>
       <c r="B4" s="110" t="s">
         <v>246</v>
       </c>
@@ -6210,7 +6297,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="189"/>
+      <c r="A5" s="200"/>
       <c r="B5" s="110" t="s">
         <v>244</v>
       </c>
@@ -6219,7 +6306,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="189"/>
+      <c r="A6" s="200"/>
       <c r="B6" s="110" t="s">
         <v>242</v>
       </c>
@@ -6228,7 +6315,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="189"/>
+      <c r="A7" s="200"/>
       <c r="B7" s="110" t="s">
         <v>240</v>
       </c>
@@ -6237,7 +6324,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="190"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="108" t="s">
         <v>238</v>
       </c>
@@ -6330,142 +6417,142 @@
       <c r="I3" s="90"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="140" t="s">
         <v>262</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="C4" s="167" t="s">
+      <c r="C4" s="142" t="s">
         <v>260</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="193" t="s">
+      <c r="E4" s="204" t="s">
         <v>258</v>
       </c>
-      <c r="F4" s="193"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="186"/>
+      <c r="F4" s="204"/>
+      <c r="G4" s="204"/>
+      <c r="H4" s="204"/>
+      <c r="I4" s="197"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="150"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="168"/>
+      <c r="A5" s="141"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="143"/>
       <c r="D5" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="194"/>
-      <c r="H5" s="194"/>
-      <c r="I5" s="164"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
+      <c r="G5" s="205"/>
+      <c r="H5" s="205"/>
+      <c r="I5" s="137"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="150"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="168"/>
+      <c r="A6" s="141"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="143"/>
       <c r="D6" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="164"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
+      <c r="G6" s="205"/>
+      <c r="H6" s="205"/>
+      <c r="I6" s="137"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="150"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="168"/>
+      <c r="A7" s="141"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="143"/>
       <c r="D7" s="113" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="194"/>
-      <c r="H7" s="194"/>
-      <c r="I7" s="164"/>
+      <c r="E7" s="205"/>
+      <c r="F7" s="205"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="205"/>
+      <c r="I7" s="137"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="150"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="168"/>
+      <c r="A8" s="141"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="143"/>
       <c r="D8" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="E8" s="194"/>
-      <c r="F8" s="194"/>
-      <c r="G8" s="194"/>
-      <c r="H8" s="194"/>
-      <c r="I8" s="164"/>
+      <c r="E8" s="205"/>
+      <c r="F8" s="205"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="205"/>
+      <c r="I8" s="137"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="150"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="168"/>
+      <c r="A9" s="141"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="143"/>
       <c r="D9" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="164"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="205"/>
+      <c r="I9" s="137"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="150"/>
-      <c r="B10" s="168"/>
-      <c r="C10" s="168"/>
+      <c r="A10" s="141"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
       <c r="D10" s="113" t="s">
         <v>255</v>
       </c>
-      <c r="E10" s="194"/>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="194"/>
-      <c r="I10" s="164"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
+      <c r="G10" s="205"/>
+      <c r="H10" s="205"/>
+      <c r="I10" s="137"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="150"/>
-      <c r="B11" s="168"/>
-      <c r="C11" s="168"/>
+      <c r="A11" s="141"/>
+      <c r="B11" s="143"/>
+      <c r="C11" s="143"/>
       <c r="D11" s="29" t="s">
         <v>254</v>
       </c>
-      <c r="E11" s="194"/>
-      <c r="F11" s="194"/>
-      <c r="G11" s="194"/>
-      <c r="H11" s="194"/>
-      <c r="I11" s="164"/>
+      <c r="E11" s="205"/>
+      <c r="F11" s="205"/>
+      <c r="G11" s="205"/>
+      <c r="H11" s="205"/>
+      <c r="I11" s="137"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
-      <c r="B12" s="168"/>
-      <c r="C12" s="168"/>
+      <c r="A12" s="141"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="143"/>
       <c r="D12" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="E12" s="194"/>
-      <c r="F12" s="194"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="194"/>
-      <c r="I12" s="164"/>
+      <c r="E12" s="205"/>
+      <c r="F12" s="205"/>
+      <c r="G12" s="205"/>
+      <c r="H12" s="205"/>
+      <c r="I12" s="137"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="192"/>
-      <c r="B13" s="191"/>
-      <c r="C13" s="191"/>
+      <c r="A13" s="203"/>
+      <c r="B13" s="202"/>
+      <c r="C13" s="202"/>
       <c r="D13" s="112" t="s">
         <v>252</v>
       </c>
-      <c r="E13" s="195"/>
-      <c r="F13" s="195"/>
-      <c r="G13" s="195"/>
-      <c r="H13" s="195"/>
-      <c r="I13" s="187"/>
+      <c r="E13" s="206"/>
+      <c r="F13" s="206"/>
+      <c r="G13" s="206"/>
+      <c r="H13" s="206"/>
+      <c r="I13" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6481,15 +6568,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6525,8 +6612,186 @@
         <v>281</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="207" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="207" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" t="s">
+        <v>304</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="180" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="124" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" s="204" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="204" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="181"/>
+      <c r="B2" s="125" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="181"/>
+      <c r="B3" s="125" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="181"/>
+      <c r="B4" s="125" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="182"/>
+      <c r="B5" s="126" t="s">
+        <v>290</v>
+      </c>
+      <c r="C5" s="206"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="180" t="s">
+        <v>297</v>
+      </c>
+      <c r="B6" s="124" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="119" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="205"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="181"/>
+      <c r="B7" s="125" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="181"/>
+      <c r="B8" s="125" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="205"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="27"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="181"/>
+      <c r="B9" s="125" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="27"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="182"/>
+      <c r="B10" s="126" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="206"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="D1:D10"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="C1:C5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="(;)">
+      <formula>NOT(ISERROR(SEARCH("(;)",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:T1 A2:B5 A6:C6 A11:T1048576 B7:C10 E2:T10">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="(">
+      <formula>NOT(ISERROR(SEARCH("(",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>"("</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>